<commit_message>
Updated URL_pattern and the others
</commit_message>
<xml_diff>
--- a/docs/capstone_docs/process/프로그램개발 진행현황(0227).xlsx
+++ b/docs/capstone_docs/process/프로그램개발 진행현황(0227).xlsx
@@ -16,14 +16,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">개발리스트!$B$3:$J$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">개발리스트!$A$1:$P$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">개발리스트!$A$1:$Q$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>메뉴명</t>
   </si>
@@ -82,10 +82,6 @@
   </si>
   <si>
     <t>관련DB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능별 상세 현황(2019.04.30현재)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -194,10 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>subject_has_professor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>signup_class
 submit
 student</t>
@@ -290,6 +282,19 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject
+subject_has_professor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발 현황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능별 상세 현황(2019.05.17현재)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -697,6 +702,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,12 +727,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1046,10 +1051,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1066,11 +1071,12 @@
     <col min="13" max="13" width="23.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="29" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -1084,87 +1090,91 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
     </row>
-    <row r="2" spans="2:15" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="27" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="31"/>
-      <c r="C3" s="24"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="33"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
       <c r="I3" s="33"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-    </row>
-    <row r="4" spans="2:15" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+    </row>
+    <row r="4" spans="2:16" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1173,30 +1183,31 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="2:16" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -1205,28 +1216,29 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
+        <v>34</v>
+      </c>
+      <c r="P5" s="15"/>
+    </row>
+    <row r="6" spans="2:16" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="23"/>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -1235,28 +1247,29 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="15"/>
+    </row>
+    <row r="7" spans="2:16" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="23"/>
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1265,28 +1278,29 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="2:16" s="1" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -1295,30 +1309,31 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="2:16" ht="33" x14ac:dyDescent="0.3">
+      <c r="B9" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1326,29 +1341,30 @@
       <c r="L9" s="6"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
+      <c r="O9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" s="15"/>
+    </row>
+    <row r="10" spans="2:16" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="23"/>
       <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1357,28 +1373,29 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="2:16" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="24"/>
+      <c r="C11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
-      <c r="C11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1387,68 +1404,69 @@
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="2:16" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>30</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="11"/>
       <c r="O12" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C15" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C16" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="M2:M3"/>
+  <mergeCells count="18">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1457,15 +1475,19 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B5:B8"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>